<commit_message>
Revise sections of Testing User Stories in TESTING.md, upload revised screenshots and update Excel Testing Sheet
</commit_message>
<xml_diff>
--- a/docs/lumiere-testing-sheet.xlsx
+++ b/docs/lumiere-testing-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pined\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1137C2-4209-4EB5-A950-1C18D3D6D67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC55719C-907E-4685-B8C7-E055DD849250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE17DBE9-D4D7-43B0-85C7-43CE4008BB7B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="48">
   <si>
     <t>Pages</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>Moto G4</t>
+  </si>
+  <si>
+    <t>feedback.html</t>
+  </si>
+  <si>
+    <t>404.html</t>
+  </si>
+  <si>
+    <t>Other Pages</t>
+  </si>
+  <si>
+    <t>Feeback for Newsletter</t>
   </si>
 </sst>
 </file>
@@ -192,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -202,6 +214,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
@@ -488,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CCA680-E4E7-4A0B-945F-5D6F0FEE729F}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -503,59 +527,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
     </row>
     <row r="3" spans="1:16" ht="36" x14ac:dyDescent="0.5">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
@@ -873,21 +897,20 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
@@ -912,7 +935,9 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -930,28 +955,56 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A13" s="2" t="s">
-        <v>37</v>
+      <c r="A13" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
@@ -998,54 +1051,26 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1063,28 +1088,56 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
+      <c r="A17" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
@@ -1131,54 +1184,26 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A19" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1196,28 +1221,56 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A21" s="2" t="s">
-        <v>26</v>
+      <c r="A21" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -1265,9 +1318,8 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3"/>
+        <v>34</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1313,8 +1365,9 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1359,56 +1412,30 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
@@ -1429,53 +1456,79 @@
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
+      <c r="A29" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1523,9 +1576,8 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3"/>
+        <v>30</v>
+      </c>
       <c r="C31" s="3" t="s">
         <v>6</v>
       </c>
@@ -1571,8 +1623,9 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
         <v>6</v>
       </c>
@@ -1617,10 +1670,12 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="3"/>
+      <c r="A33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
@@ -1665,83 +1720,80 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A34" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P34" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A35" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A36" s="2" t="s">
-        <v>31</v>
+      <c r="A36" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>2</v>
+      </c>
       <c r="C37" s="3" t="s">
         <v>6</v>
       </c>
@@ -1786,59 +1838,29 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P38" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -1855,24 +1877,119 @@
       <c r="P39" s="3"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
+      <c r="A40" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="A42" s="2"/>
+      <c r="A42" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A44" s="7">
+        <v>404</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P44" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>